<commit_message>
Add one more subscription, and add the debug output email body HTML file.
</commit_message>
<xml_diff>
--- a/files/subscriptions.xlsx
+++ b/files/subscriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b064b1ad65f4371e/Training/PyProjects/EmailNewsFeed/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{779A076F-F1A2-43DE-9E8C-3D1A8146F634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54F90A44-B38C-4E12-AA0D-72C29C6E8960}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{779A076F-F1A2-43DE-9E8C-3D1A8146F634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D97EC3E8-9C86-45BE-B60C-67725A08F469}"/>
   <bookViews>
     <workbookView xWindow="4785" yWindow="1170" windowWidth="20685" windowHeight="14355" xr2:uid="{29F88AFA-134A-4825-963A-01402C9FA212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Steven</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Ukraine, Micropython, Tesla, Subaru</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>s_elkind@yahoo.com</t>
+  </si>
+  <si>
+    <t>Ukraine, Micropython, Tesla, Subaru, Lindsey Stirling</t>
   </si>
 </sst>
 </file>
@@ -144,10 +156,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D64F823-35F0-47B3-A66E-373B78D5E141}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +466,7 @@
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,12 +511,27 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{96CCB98E-0FC5-4303-A60C-65BA57EA79B0}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{7068ADA3-A5BA-4820-9CE4-2D5461A56272}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{0C865329-5945-4966-A061-C046DF52B6E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>